<commit_message>
multiple random starting points
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Paper / book</t>
   </si>
@@ -61,6 +61,39 @@
   </si>
   <si>
     <t>Great: this is exactly the oscillation pattern learning gives you</t>
+  </si>
+  <si>
+    <t>D'Acunto, Hoang, Weber 2020 WP</t>
+  </si>
+  <si>
+    <t>With a diff-in-diff, they show that households' expectations react to unconventional fiscal pol (telling them about higher taxes in the future), but not to forward guidance. The difference is due to what mechanism they understand.</t>
+  </si>
+  <si>
+    <t>Coibion, Goro, Weber 2020 WP</t>
+  </si>
+  <si>
+    <t>Does policy communication during Covid influence expectations and spending plans of households? In short, no.</t>
+  </si>
+  <si>
+    <t>Interesting for me b/c it suggests that expectations can't incorporate communication.</t>
+  </si>
+  <si>
+    <t>Bottan, Perez-Truglia 2020 WP</t>
+  </si>
+  <si>
+    <t>HHs do incorporate info about home prices and it strongly affects their decision when to sell</t>
+  </si>
+  <si>
+    <t>expectations can incorporate info about individual stuff -&gt; Preston is right, HHs understand their idiosyncratic circumstances, but not necessarily the aggregate model</t>
+  </si>
+  <si>
+    <t>Bianchi, Ludvigson, Mai 2020 WP</t>
+  </si>
+  <si>
+    <t>A horserace of theories seems to suggests that individuals fluctuate between optimism and pessimism (ie over- or undershooting) again, resembling learning</t>
+  </si>
+  <si>
+    <t>provide a new measure of expectational errors in survey responses. Nice lit review. Interesting: their benchmark isn't RE: it's a machine-learning forecasting algorithm. Already this speaks volumes as to how reasonable learning is.</t>
   </si>
 </sst>
 </file>
@@ -483,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -550,6 +583,47 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
cleaned up CEMP and CUSUM crits, scalar and vector
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Paper / book</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>provide a new measure of expectational errors in survey responses. Nice lit review. Interesting: their benchmark isn't RE: it's a machine-learning forecasting algorithm. Already this speaks volumes as to how reasonable learning is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coibion, Georgarakos, Goro, Weber 2020 WP, Forward Guidance and Household Expectations </t>
+  </si>
+  <si>
+    <t>Support models with agents with limited capacity to collect and process information e.g Woodford 2018, Gabaix 2019, Fahri and Werning 2018</t>
+  </si>
+  <si>
+    <t>Survey on US HHs and RCT: 1.) HHs uninformed about market interests rates 2.) When we provide info about current and one-period ahead interest rates, has large effects on beliefs 3) When we provide info on interest rates far out in the future, it has a very small effect</t>
   </si>
 </sst>
 </file>
@@ -516,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -524,13 +533,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="88.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -548,7 +557,7 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -558,8 +567,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -570,7 +579,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="30">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -584,7 +593,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -592,7 +601,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -603,7 +612,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -614,7 +623,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -622,6 +631,17 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Peter meeting on averaging cross-sections in SMM
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -36,12 +36,6 @@
     <t>Conclusions</t>
   </si>
   <si>
-    <t>PS and CB disagree about expected AD. Disagreement + learning --&gt; disagreement about future interest rates.</t>
-  </si>
-  <si>
-    <t>Market perceives monpol "mistakes: and the Fed partially accomodates the market's view</t>
-  </si>
-  <si>
     <t>Andrade, Coibion, Gautier, Gorodnichenko 2020 WP</t>
   </si>
   <si>
@@ -103,6 +97,47 @@
   </si>
   <si>
     <t>Survey on US HHs and RCT: 1.) HHs uninformed about market interests rates 2.) When we provide info about current and one-period ahead interest rates, has large effects on beliefs 3) When we provide info on interest rates far out in the future, it has a very small effect</t>
+  </si>
+  <si>
+    <t>PS and CB disagree about expected AD (even after FOMC announcements). Disagreement + learning --&gt; disagreement about future interest rates. Their "(relative) confidence" is their analogy of my gain. Btw: they do have endog. Volatility, of course!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Market perceives monpol "mistakes: and the Fed partially accomodates the market's view. Annette Vissing-Jørgensen in her discussion said that we need a a model about the disagreement about the Fed's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -115,6 +150,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -528,7 +564,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -556,92 +592,92 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="30">
       <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45">
       <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did a run w/o convexity moment, doesn't seem to work well, and did a run with it on real data, saved results in materials36.tex
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Paper / book</t>
   </si>
@@ -122,7 +122,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -139,18 +138,41 @@
       <t>function.</t>
     </r>
   </si>
+  <si>
+    <t>Afrouzi Yang 2020 WP?</t>
+  </si>
+  <si>
+    <t>dynamic rational inattention solving software + idea that Phillips curve has become flat because monpol more hawkish, and more hawkish monpol anchors expectations</t>
+  </si>
+  <si>
+    <t>I can relate my endogenous gain to their "time-dependent Kalman gain" which is what matters for the slope of the Phillips curve: you choose a higher KG when environment more volatile (load more on shocks i.e choose to acquire more info), steeper PC. When inflation coefficient of TR high, you choose low Kalman gain because the environment becomes less volatile, PC becomes flat.</t>
+  </si>
+  <si>
+    <t>But as Woodford pointed out at NBER SI, there is no concept of long-run expectations, and thus of anchoring.</t>
+  </si>
+  <si>
+    <t>Coibion, Goro, Weber 2020 WP, Monetary Policy Communications and their Effects on Household Inflation Expectations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCT with info treatment on HH infl expectations survey. </t>
+  </si>
+  <si>
+    <t>Main result: simple messages (current inflation, Fed decision, Fed forecast) are the most effective on having an effect on inflation expectations.</t>
+  </si>
+  <si>
+    <t>Ricardo Reis discussion: Past inflation and inflation target have the same effect on E —&gt; surprising given that one is varying and the other constant —&gt; me: not if the other is not perceived to be constant</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -176,6 +198,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF444444"/>
+      <name val=".SFUIText"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,7 +237,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -224,6 +251,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -561,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -572,9 +603,10 @@
     <col min="1" max="1" width="35.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="88.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -584,7 +616,7 @@
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3"/>
@@ -624,7 +656,7 @@
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -679,6 +711,40 @@
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="60">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:8" ht="22">
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
did 1) nice speedups 2) runs with 100K convexity weight 3) real data runs with N=1000
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Paper / book</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Ricardo Reis discussion: Past inflation and inflation target have the same effect on E —&gt; surprising given that one is varying and the other constant —&gt; me: not if the other is not perceived to be constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey of Consumers bias is on a scale of [-4,4] (difference between machine and survey respondent forecast) —&gt; that might be a reasonable range for me </t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -690,7 +693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -699,6 +702,9 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45">

</xml_diff>

<commit_message>
ridge regression - why you should standardize the regressor matrix
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Paper / book</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t xml:space="preserve">Survey of Consumers bias is on a scale of [-4,4] (difference between machine and survey respondent forecast) —&gt; that might be a reasonable range for me </t>
+  </si>
+  <si>
+    <t>Angeletos, Lian 2020 WP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why do demand shocks drive BCs? Theory of 1) intertemporal substi in production 2) bounded rationality in consumption. </t>
+  </si>
+  <si>
+    <t>1) allows supply to respond to demand w.o price stickiness, 2) introduces a 'confidence multipllier': a positive feedback loop between real activity and expectations</t>
+  </si>
+  <si>
+    <t>I didn’t save a copy of this paper. It's called Confidence and The Propagation of Demand Shocks</t>
   </si>
 </sst>
 </file>
@@ -597,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,6 +758,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="13" spans="1:8">
       <c r="D13"/>
     </row>

</xml_diff>

<commit_message>
reading bordalo and hebden et al
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="69200" yWindow="-3880" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Paper / book</t>
   </si>
@@ -176,6 +176,24 @@
   </si>
   <si>
     <t>I didn’t save a copy of this paper. It's called Confidence and The Propagation of Demand Shocks</t>
+  </si>
+  <si>
+    <t>explain that individuals overreact to their news using representativeness heuristic. When everyone overreacts, the average underreacts to news.</t>
+  </si>
+  <si>
+    <t>cannot account for time-varying over and underreaction, silent on LR-E, both of which is to say that it cannot account for anchoring</t>
+  </si>
+  <si>
+    <t>diagnostic expectations (Bordalo et al, 2018 (unpublished) and 2018)</t>
+  </si>
+  <si>
+    <t>Hebden et al 2020</t>
+  </si>
+  <si>
+    <t>Makeup strategies work well when expectations understand, believe and act on the CB's policy commitment. Otherwise, costly action is necessary (as in Goodfriend and King)</t>
+  </si>
+  <si>
+    <t>Long-run expectations seem anchored generally, but in surveys, a majority of respondents does revise its expectations for persistent deviations . In survey data, inflation expectations, even individual ones, generally underreact to news.</t>
   </si>
 </sst>
 </file>
@@ -609,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -772,10 +790,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="30">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" ht="22">
+    <row r="14" spans="1:8" ht="46">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D14" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to find more evidence of unanchoring
so far it's not great I don't think
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Paper / book</t>
   </si>
@@ -194,6 +194,27 @@
   </si>
   <si>
     <t>Long-run expectations seem anchored generally, but in surveys, a majority of respondents does revise its expectations for persistent deviations . In survey data, inflation expectations, even individual ones, generally underreact to news.</t>
+  </si>
+  <si>
+    <t>Model of costly reasoning to update beliefs about optimal mapping of econ states to actions.</t>
+  </si>
+  <si>
+    <t>Key result: agents reason more about a state when its unusual --&gt; state/history-dependent behavior with 'learning traps': endogenous familiar regions of state space where behavior appears to follow past experience based heuristics. Traps have empirically desirable properties: MPC higher, hand-to-mout more frequent and persistent and more welath inequality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In an incomplete market setting, a learning-type setting produces desirable empirical features. </t>
+  </si>
+  <si>
+    <t>Ilut &amp; Valchev 2020 WP, Economic Agents as Imperfect Problem Solvers</t>
+  </si>
+  <si>
+    <t>Candia, Coibion &amp; Goro 2020, Communication and the Beliefs of Economic Agents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look at surveys of expectations to examine how beliefs affect actions. Info provision about inflation can have opposite effects on actions depending on whether agents interpret them as supply  or demand side. As opposed to profi forecasters, HHs (but also many firms) tend to interpret inflation as supply-side, thus leading to actions that depress the economy. </t>
+  </si>
+  <si>
+    <t>This may have been what Jenny mentioned. No b/c that was a JMP… and also in that JMP firms interpreted inflation as a demand shock, so it was expansionary</t>
   </si>
 </sst>
 </file>
@@ -625,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -814,6 +835,31 @@
       </c>
       <c r="D14" s="8"/>
     </row>
+    <row r="15" spans="1:8" ht="60">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
minor changes, typos etc in prezi
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Paper / book</t>
   </si>
@@ -122,7 +122,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -223,6 +222,18 @@
   <si>
     <t xml:space="preserve">Use daily survey of US households to see whether their expectations are affected by announcing an average inflation targeting framework. In short, no. A minority states that they've heard news, but this affect fades in a few days. Moreover, their expectations do not change after hearing the news, indicating that they didn't understand it. </t>
   </si>
+  <si>
+    <t>Afrouzi et al WP 2020 working memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cgain learning and diagnostic overreact too little. A main feature in the data is the variation of overreaction across different settings, and that overreaction appears to be stronger when the forecast horizon is longer (see Bouchaud et al. (2019) and Bordalo et al. (2019) for evidence from analyst earnings forecasts, as well as Brooks, Katz and Lustig (2018), Wang (2019), and d’Arienzo (2020) for evidence from interest rate forecasts). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment of expectations, documenting new evidence. They develop a working memory model, where ppl estimate long-run means of the process subject to a cost of utilizing past information. </t>
+  </si>
+  <si>
+    <t>Should be my standard response to the diagnostic E question.</t>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +245,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -654,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,12 +878,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="75">
+      <c r="A18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Brian meeting, Eusepi meeting, Jenny meeting and quick fixes to technical prezi
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Paper / book</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>Should be my standard response to the diagnostic E question.</t>
+  </si>
+  <si>
+    <t>Hazell et al 2020 WP (w/ Nakamura and Steinsson)</t>
+  </si>
+  <si>
+    <t>Estimate slope of PC, show it's always been flat, even early 1980s. No missing disinflation or missing reinflation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results imply that drop in core inflation in 1980s due to shifting expectations about long-run mon pol as opposed to a steep Phillips curve, and greater stability of inflation since 1990s is mostly due to long-run infl expectations becoming more firmly anchored. </t>
+  </si>
+  <si>
+    <t>Boutros et al 2020 WP</t>
+  </si>
+  <si>
+    <t>Use forecasts of one-year S&amp;P500 returns to track how beliefs of chief financial officers (CFOs) evolve. CFOs' beliefs are unbiased on average, but have too narrow Cis (they refer to this as miscalibration). When returns realized fall outside the Cis, the CIs widen.</t>
+  </si>
+  <si>
+    <t>Interpret this as consistent with Bayesian learning. But the magnitude of updating is too small. They say it is "dampened by strong conviction in beliefs in the initial miscalibration" and as a result, miscalibration persists. I.e. priors are really strong.</t>
   </si>
 </sst>
 </file>
@@ -664,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -900,6 +918,28 @@
         <v>59</v>
       </c>
     </row>
+    <row r="19" spans="1:4" ht="45">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
lit and general interest intro
</commit_message>
<xml_diff>
--- a/literature/record_empirical_features_expectations.xlsx
+++ b/literature/record_empirical_features_expectations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="69200" yWindow="-3880" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="33520" yWindow="3240" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Paper / book</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>Interpret this as consistent with Bayesian learning. But the magnitude of updating is too small. They say it is "dampened by strong conviction in beliefs in the initial miscalibration" and as a result, miscalibration persists. I.e. priors are really strong.</t>
+  </si>
+  <si>
+    <t>Grigoli et al 2020 WP</t>
+  </si>
+  <si>
+    <t>Use dispersion of infl forecasts as proxy for extent of anchoring, and find that this goes up after a mon pol surprise. Rationalize using a model with RE and sticky info.</t>
+  </si>
+  <si>
+    <t>Slobodyan Wouters, 2012, 2017</t>
+  </si>
+  <si>
+    <t>estimate medium-scale DSGE with adaptive learning, fits much better than RE</t>
   </si>
 </sst>
 </file>
@@ -682,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -940,6 +952,22 @@
         <v>65</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="30">
+      <c r="A21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>